<commit_message>
change unit in example 8151fac5b289ac7fbb0fea8c070596bd72539cca
</commit_message>
<xml_diff>
--- a/nr-add-lipids/ig/StructureDefinition-mesures-observation-cholesterol-hdl.xlsx
+++ b/nr-add-lipids/ig/StructureDefinition-mesures-observation-cholesterol-hdl.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-11T16:39:06+00:00</t>
+    <t>2024-12-11T17:02:02+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1028,7 +1028,7 @@
     <t>There are many representations for units of measure and in many contexts, particular representations are fixed and required. I.e. mcg for micrograms.</t>
   </si>
   <si>
-    <t>g/L</t>
+    <t>mmol/L</t>
   </si>
   <si>
     <t>Quantity.unit</t>

</xml_diff>

<commit_message>
add ref range 4b02c9fb217dbb5c3e7b718f8ab18b4327b080d3
</commit_message>
<xml_diff>
--- a/nr-add-lipids/ig/StructureDefinition-mesures-observation-cholesterol-hdl.xlsx
+++ b/nr-add-lipids/ig/StructureDefinition-mesures-observation-cholesterol-hdl.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-13T13:39:29+00:00</t>
+    <t>2024-12-13T13:45:52+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -7987,7 +7987,7 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>93</v>

</xml_diff>